<commit_message>
added summer time with EEPROm seving
</commit_message>
<xml_diff>
--- a/1 - System Docs/DEV_notes_REV2.xlsx
+++ b/1 - System Docs/DEV_notes_REV2.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\01_GIT_REPOS\A_light_2\1 - System Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="changelog" sheetId="9" r:id="rId1"/>
@@ -25,7 +20,7 @@
     <sheet name="HTTP_replace function" sheetId="5" r:id="rId11"/>
     <sheet name="TODO" sheetId="11" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="637">
   <si>
     <t>normal</t>
   </si>
@@ -2044,6 +2039,24 @@
   </si>
   <si>
     <t>added more delays to ext trigger</t>
+  </si>
+  <si>
+    <t>/summertime_on</t>
+  </si>
+  <si>
+    <t>/summertime_off</t>
+  </si>
+  <si>
+    <t>//V1.1 added clock show yellow while in alarm shine mode</t>
+  </si>
+  <si>
+    <t>//V1.2 added internet time NTP client, added summer time commands and menu on default webpage</t>
+  </si>
+  <si>
+    <t>removed to zeros by cleareeprom</t>
+  </si>
+  <si>
+    <t>Summer time ON (0b1)/OFF (0b0)</t>
   </si>
 </sst>
 </file>
@@ -2203,18 +2216,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normálne" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2232,7 +2245,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="sk-SK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2244,6 +2257,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2446,11 +2460,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166908712"/>
-        <c:axId val="166903224"/>
+        <c:axId val="204726848"/>
+        <c:axId val="204727424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166908712"/>
+        <c:axId val="204726848"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2498,6 +2512,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2506,26 +2521,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
@@ -2564,12 +2559,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166903224"/>
+        <c:crossAx val="204727424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166903224"/>
+        <c:axId val="204727424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2615,6 +2610,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2623,26 +2619,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2681,7 +2657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166908712"/>
+        <c:crossAx val="204726848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2733,7 +2709,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="sk-SK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2770,6 +2746,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2778,26 +2755,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3293,11 +3250,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="166905184"/>
-        <c:axId val="166907536"/>
+        <c:axId val="181330944"/>
+        <c:axId val="204730304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166905184"/>
+        <c:axId val="181330944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3339,7 +3296,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166907536"/>
+        <c:crossAx val="204730304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3347,7 +3304,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166907536"/>
+        <c:axId val="204730304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3398,7 +3355,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166905184"/>
+        <c:crossAx val="181330944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3412,6 +3369,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3481,7 +3439,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="sk-SK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3493,6 +3451,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3682,11 +3641,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166909496"/>
-        <c:axId val="166909888"/>
+        <c:axId val="204732032"/>
+        <c:axId val="204732608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166909496"/>
+        <c:axId val="204732032"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3734,6 +3693,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3742,26 +3702,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
@@ -3800,12 +3740,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166909888"/>
+        <c:crossAx val="204732608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166909888"/>
+        <c:axId val="204732608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3851,6 +3791,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3859,26 +3800,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3917,7 +3838,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166909496"/>
+        <c:crossAx val="204732032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3969,7 +3890,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="sk-SK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4011,6 +3932,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4019,26 +3941,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -4220,11 +4122,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166904400"/>
-        <c:axId val="166910280"/>
+        <c:axId val="204808192"/>
+        <c:axId val="204808768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166904400"/>
+        <c:axId val="204808192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4281,12 +4183,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166910280"/>
+        <c:crossAx val="204808768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166910280"/>
+        <c:axId val="204808768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4343,7 +4245,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166904400"/>
+        <c:crossAx val="204808192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4357,6 +4259,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7049,7 +6952,7 @@
         <xdr:cNvPr id="2" name="Graf 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{433795F3-C114-499C-83D8-08A11B52284E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{433795F3-C114-499C-83D8-08A11B52284E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7087,7 +6990,7 @@
         <xdr:cNvPr id="3" name="Obdĺžnik 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D084D97-70BA-4174-8B55-DFFEE60CFFE6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6D084D97-70BA-4174-8B55-DFFEE60CFFE6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7155,7 +7058,7 @@
         <xdr:cNvPr id="4" name="Obdĺžnik 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1704C95-B726-4671-B77E-473DB2232F5A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C1704C95-B726-4671-B77E-473DB2232F5A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7223,7 +7126,7 @@
         <xdr:cNvPr id="5" name="Obdĺžnik 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F946AAD-1FE9-49C5-845A-53D22C94675B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2F946AAD-1FE9-49C5-845A-53D22C94675B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7291,7 +7194,7 @@
         <xdr:cNvPr id="6" name="Rovná spojnica 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{193BA6DB-C7ED-4B73-B27C-AA4251CC2D37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{193BA6DB-C7ED-4B73-B27C-AA4251CC2D37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7344,7 +7247,7 @@
         <xdr:cNvPr id="7" name="Rovná spojnica 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{001CC3D6-3C14-4E8F-B319-09396A0D9119}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{001CC3D6-3C14-4E8F-B319-09396A0D9119}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7396,7 +7299,7 @@
         <xdr:cNvPr id="8" name="Rovná spojnica 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41C38ACC-16BE-40BE-8783-27B0B58F9ADD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{41C38ACC-16BE-40BE-8783-27B0B58F9ADD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7781,7 +7684,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7789,10 +7692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7853,8 +7756,21 @@
       <c r="B9">
         <v>200205</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="14" t="s">
         <v>630</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="14" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>20201222</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>634</v>
       </c>
     </row>
   </sheetData>
@@ -15153,10 +15069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15250,8 +15166,19 @@
         <v>588</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>632</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18203,20 +18130,21 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>561</v>
       </c>
@@ -18227,88 +18155,128 @@
         <v>564</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>566</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="16" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>562</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>31</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>21</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>567</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="15" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>562</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>95</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>256</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>568</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="15" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>562</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="14"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="16"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>296</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="14"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>300</v>
+      </c>
+      <c r="B13" t="s">
+        <v>636</v>
+      </c>
+      <c r="C13" t="s">
+        <v>553</v>
+      </c>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>511</v>
+      </c>
+      <c r="D16" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="D2:D16"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C2:C4"/>

</xml_diff>